<commit_message>
vault backup: 2025-02-27 11:49:22
</commit_message>
<xml_diff>
--- a/00 Attachments/Complemento Presupuesto de Ventas Formato.xlsx
+++ b/00 Attachments/Complemento Presupuesto de Ventas Formato.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb906e424dbf4747/Documentos/Fundamentos de Administración y Análisis Financiero 2025 Industrial 1er. Semestre/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pca20\git\apuntes_url\00 Attachments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BB0A570-C59F-475F-9995-B66ECBC03E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7075F5AF-DF31-44EA-8E22-D8E3BBBE274F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{94973479-FC48-4CC7-A4EE-520F84DA9A8C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{94973479-FC48-4CC7-A4EE-520F84DA9A8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Cuadro Presupuesto de Ventas" sheetId="1" r:id="rId1"/>
@@ -200,7 +200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -214,16 +214,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -239,7 +241,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -537,110 +539,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B64E4ED6-35E3-4214-8D52-306425652437}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1"/>
-    <col min="2" max="3" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="50.6640625" customWidth="1"/>
+    <col min="2" max="3" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="10">
+        <v>-800000</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="10">
+        <v>500000</v>
+      </c>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="11">
+        <v>600000</v>
+      </c>
+      <c r="C6" s="11">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10">
+        <v>5300000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="10"/>
+      <c r="C8" s="11">
+        <v>-265000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10">
+        <v>5035000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10">
+        <v>503500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="10"/>
+      <c r="C11" s="12">
+        <v>5538500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
@@ -657,19 +679,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9253A153-430E-4DA0-B074-2582A93D5E54}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1">
         <v>2024</v>
       </c>
@@ -680,127 +702,187 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>0.08</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="5">
+        <v>11070000</v>
+      </c>
+      <c r="D2" s="5">
+        <f>+C2*B2</f>
+        <v>885600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>0.09</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="9">
+        <v>11070000</v>
+      </c>
+      <c r="D3" s="9">
+        <f t="shared" ref="D3:D13" si="0">+C3*B3</f>
+        <v>996300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>0.1</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="9">
+        <v>11070000</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" si="0"/>
+        <v>1107000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>0.11</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="9">
+        <v>11070000</v>
+      </c>
+      <c r="D5" s="9">
+        <f t="shared" si="0"/>
+        <v>1217700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="9">
+        <v>11070000</v>
+      </c>
+      <c r="D6" s="9">
+        <f t="shared" si="0"/>
+        <v>774900.00000000012</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>0.06</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="9">
+        <v>11070000</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" si="0"/>
+        <v>664200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>0.05</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="9">
+        <v>11070000</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" si="0"/>
+        <v>553500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>0.09</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="9">
+        <v>11070000</v>
+      </c>
+      <c r="D9" s="9">
+        <f t="shared" si="0"/>
+        <v>996300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>0.115</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="9">
+        <v>11070000</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" si="0"/>
+        <v>1273050</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="9">
+        <v>11070000</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" si="0"/>
+        <v>929880</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>0.05</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="9">
+        <v>11070000</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" si="0"/>
+        <v>553500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="4">
         <v>0.10100000000000001</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="9">
+        <v>11070000</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" si="0"/>
+        <v>1118070</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -809,9 +891,12 @@
         <v>1</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="D14" s="7">
+        <f>+SUM(D2:D13)</f>
+        <v>11070000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>